<commit_message>
Modified the videos that are added, to ensure that they are >5k and have captions enabled. Then from the video ids used the youtube-transcription-api to get teh transcripts of the videos, and used WebShare to create rotating residential proxy servers to avoid being blocked by YouTube
</commit_message>
<xml_diff>
--- a/Documentation/Weekly Sprint Reports.xlsx
+++ b/Documentation/Weekly Sprint Reports.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawye\CS Senior Final Project\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawye\YouTube-Intelligence-Platform\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C33051C-D8B7-4338-A5EC-A6E6FCDB7BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DE01B8-9C10-4463-924A-B3752589A8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39645" yWindow="3780" windowWidth="14400" windowHeight="7275" xr2:uid="{507938F6-A526-48DD-A146-6D86B46D0651}"/>
+    <workbookView xWindow="4770" yWindow="1630" windowWidth="14400" windowHeight="7270" xr2:uid="{507938F6-A526-48DD-A146-6D86B46D0651}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -35,15 +35,96 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Story name</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Issue Type</t>
+  </si>
+  <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t># hrs</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Completion Date</t>
+  </si>
+  <si>
+    <t>Epic (Optional)</t>
+  </si>
+  <si>
+    <t>Story</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Whole Team</t>
+  </si>
+  <si>
+    <t>Create project proposal, research technology and APIs</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Create project proposal</t>
+  </si>
+  <si>
+    <t>Research YouTube API</t>
+  </si>
+  <si>
+    <t>Whole Team (specifically Data Scientists and Back-end engineers</t>
+  </si>
+  <si>
+    <t>Create GitHub Repo</t>
+  </si>
+  <si>
+    <t>Sawyer</t>
+  </si>
+  <si>
+    <t>10min</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +143,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,14 +507,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5DBE3B-10DC-45DA-867D-5D449B91B27F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3">
+        <v>46062</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3">
+        <v>46062</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3">
+        <v>46062</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3">
+        <v>46062</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>